<commit_message>
Ajuste nos testes de previsão inicial das deduções da receita
</commit_message>
<xml_diff>
--- a/report-mun.xlsx
+++ b/report-mun.xlsx
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>480031.68</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>480031.68</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -642,7 +642,7 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>480031.68</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -650,7 +650,7 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>480031.68</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>4413781.71</v>
+        <v>4053505.25</v>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>12750182.8</v>
+        <v>12695902.02</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -827,7 +827,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>4413781.71</v>
+        <v>4053505.25</v>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -835,10 +835,10 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>4107786.030000001</v>
+        <v>4053505.25</v>
       </c>
       <c r="O10" t="n">
-        <v>305995.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>2627951.08</v>
+        <v>3236811.88</v>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>2627456.08</v>
+        <v>3236811.88</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1012,7 +1012,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>2627951.08</v>
+        <v>3236811.88</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1020,10 +1020,10 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>2627456.08</v>
+        <v>3236811.88</v>
       </c>
       <c r="O15" t="n">
-        <v>495</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>413094.04</v>
+        <v>387874.28</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>107098.36</v>
+        <v>100559.88</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>306490.68</v>
+        <v>287314.4</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
@@ -1236,7 +1236,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>413094.04</v>
+        <v>387874.28</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -1244,10 +1244,10 @@
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>413589.04</v>
+        <v>387874.28</v>
       </c>
       <c r="O21" t="n">
-        <v>-495</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>686664.0600000001</v>
+        <v>1192366.06</v>
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>686664.0600000001</v>
+        <v>1192366.06</v>
       </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
@@ -1489,7 +1489,7 @@
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>686664.0600000001</v>
+        <v>1192366.06</v>
       </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
@@ -1497,7 +1497,7 @@
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
-        <v>686664.0600000001</v>
+        <v>1192366.06</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
@@ -1673,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>70000</v>
+        <v>251338.26</v>
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>70000</v>
+        <v>251338.26</v>
       </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
@@ -1777,7 +1777,7 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>70000</v>
+        <v>251338.26</v>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
@@ -1785,7 +1785,7 @@
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="n">
-        <v>70000</v>
+        <v>251338.26</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -1961,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>248508.27</v>
+        <v>701458.4</v>
       </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
-        <v>248508.27</v>
+        <v>701458.4</v>
       </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
@@ -2065,7 +2065,7 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>248508.27</v>
+        <v>701458.4</v>
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
@@ -2073,7 +2073,7 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="n">
-        <v>248508.27</v>
+        <v>701458.4</v>
       </c>
       <c r="O44" t="n">
         <v>0</v>

</xml_diff>